<commit_message>
work with table widths
</commit_message>
<xml_diff>
--- a/DocumentPages/TimeSheets/9-2017.xlsx
+++ b/DocumentPages/TimeSheets/9-2017.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blaine/Documents/school/C445/Time-sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wbcod\sch\P445\DocumentPages\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="18960" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MR" sheetId="1" r:id="rId1"/>
     <sheet name="BP" sheetId="2" r:id="rId2"/>
     <sheet name="JO" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -138,8 +138,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -151,6 +151,13 @@
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -174,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -197,6 +204,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -207,6 +227,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -474,23 +497,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="22.375" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+    <col min="4" max="4" width="21.875" customWidth="1"/>
+    <col min="6" max="6" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <v>42979</v>
       </c>
@@ -522,7 +545,7 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>42983</v>
       </c>
@@ -533,7 +556,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>42986</v>
       </c>
@@ -544,7 +567,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>42987</v>
       </c>
@@ -555,7 +578,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>42995</v>
       </c>
@@ -566,7 +589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>43004</v>
       </c>
@@ -583,23 +606,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.125" customWidth="1"/>
     <col min="3" max="3" width="46.5" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.875" customWidth="1"/>
+    <col min="6" max="6" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -616,7 +639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <v>42980</v>
       </c>
@@ -631,7 +654,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>42982</v>
       </c>
@@ -642,7 +665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>42986</v>
       </c>
@@ -653,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>42987</v>
       </c>
@@ -664,7 +687,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>42990</v>
       </c>
@@ -675,7 +698,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>42992</v>
       </c>
@@ -686,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>42996</v>
       </c>
@@ -697,7 +720,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>43001</v>
       </c>
@@ -708,7 +731,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>43002</v>
       </c>
@@ -725,152 +748,248 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="51.5" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="25.875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="51.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11" style="9"/>
+    <col min="6" max="6" width="20.5" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="3">
+    <row r="2" spans="1:6" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12">
         <v>42980</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="10">
         <v>2.25</v>
       </c>
-      <c r="F2" s="4">
+      <c r="E2" s="11"/>
+      <c r="F2" s="10">
         <f>SUM(D2:D20)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="3">
+    <row r="3" spans="1:6" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12">
         <v>42986</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="3">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12">
         <v>42987</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="3">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12">
         <v>42990</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="3">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12">
         <v>42991</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="6">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="13">
         <v>42993</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="6">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="13">
         <v>42997</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="11">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="6">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="13">
         <v>43000</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="11">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="6">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="13">
         <v>43007</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="11">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="6">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="13">
         <v>43008</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="11">
         <v>1.5</v>
       </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>